<commit_message>
Fix typo in Power_BusInfo (-> v0.0.3r)
</commit_message>
<xml_diff>
--- a/examples/Power_BusInfo.xlsx
+++ b/examples/Power_BusInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92498DF-FDD7-42EB-A230-33BBC5CE6B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDAE8F6-268A-456C-8EE0-6971AB99BA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarioA" sheetId="111" r:id="rId1"/>
@@ -364,9 +364,6 @@
     <t>pBusB</t>
   </si>
   <si>
-    <t>Suceptance B connected to node</t>
-  </si>
-  <si>
     <t>Conductance G connected to node</t>
   </si>
   <si>
@@ -484,13 +481,16 @@
     <t>Year where it is decommissioned (31.12.xxxx)</t>
   </si>
   <si>
-    <t>v0.0.3</t>
-  </si>
-  <si>
     <t>[0, 1]</t>
   </si>
   <si>
     <t>Whether node is relevant for end result (1) or not (0)</t>
+  </si>
+  <si>
+    <t>Susceptance B connected to node</t>
+  </si>
+  <si>
+    <t>v0.0.3r</t>
   </si>
 </sst>
 </file>
@@ -1140,15 +1140,15 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>18</v>
@@ -1175,33 +1175,33 @@
         <v>2</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>19</v>
@@ -1225,31 +1225,31 @@
         <v>35</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>48</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -1273,97 +1273,97 @@
         <v>34</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="J5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>75</v>
-      </c>
       <c r="M5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="O5" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="P6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>3</v>
@@ -1396,13 +1396,13 @@
         <v>16</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="12">
         <v>220</v>
@@ -1448,10 +1448,10 @@
         <v>1</v>
       </c>
       <c r="P8" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1461,7 +1461,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="12">
         <v>220</v>
@@ -1497,10 +1497,10 @@
         <v>1</v>
       </c>
       <c r="P9" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q9" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -1512,7 +1512,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="12">
         <v>220</v>
@@ -1548,10 +1548,10 @@
         <v>1</v>
       </c>
       <c r="P10" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q10" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q10" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
@@ -1563,7 +1563,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="12">
         <v>220</v>
@@ -1599,10 +1599,10 @@
         <v>1</v>
       </c>
       <c r="P11" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q11" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q11" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="12">
         <v>220</v>
@@ -1648,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="P12" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q12" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q12" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1661,7 +1661,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="12">
         <v>220</v>
@@ -1697,10 +1697,10 @@
         <v>1</v>
       </c>
       <c r="P13" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q13" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="12">
         <v>220</v>
@@ -1746,10 +1746,10 @@
         <v>1</v>
       </c>
       <c r="P14" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q14" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="12">
         <v>220</v>
@@ -1795,10 +1795,10 @@
         <v>1</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q15" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="12">
         <v>220</v>
@@ -1844,24 +1844,24 @@
         <v>1</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q16" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="22"/>
       <c r="C17" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="12">
         <v>220</v>
@@ -1897,10 +1897,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q17" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q17" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1919,9 +1919,9 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="O6" sqref="O6"/>
-      <selection pane="topRight" activeCell="O6" sqref="O6"/>
-      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
+      <selection activeCell="H6" sqref="H6"/>
+      <selection pane="topRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -1940,15 +1940,15 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>18</v>
@@ -1975,33 +1975,33 @@
         <v>2</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>19</v>
@@ -2025,31 +2025,31 @@
         <v>35</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>48</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -2073,97 +2073,97 @@
         <v>34</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="J5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>75</v>
-      </c>
       <c r="M5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="O5" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="L6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="M6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="P6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="Q6" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>3</v>
@@ -2196,13 +2196,13 @@
         <v>16</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2212,7 +2212,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="12">
         <v>220</v>
@@ -2248,10 +2248,10 @@
         <v>1</v>
       </c>
       <c r="P8" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2261,7 +2261,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="12">
         <v>220</v>
@@ -2297,10 +2297,10 @@
         <v>1</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q9" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -2312,7 +2312,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="12">
         <v>220</v>
@@ -2348,10 +2348,10 @@
         <v>1</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q10" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
@@ -2363,7 +2363,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="12">
         <v>220</v>
@@ -2399,10 +2399,10 @@
         <v>0</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q11" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2412,7 +2412,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="12">
         <v>220</v>
@@ -2448,10 +2448,10 @@
         <v>0</v>
       </c>
       <c r="P12" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q12" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q12" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="12">
         <v>220</v>
@@ -2497,10 +2497,10 @@
         <v>0</v>
       </c>
       <c r="P13" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q13" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q13" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2510,7 +2510,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="12">
         <v>220</v>
@@ -2546,10 +2546,10 @@
         <v>0</v>
       </c>
       <c r="P14" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q14" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="12">
         <v>220</v>
@@ -2595,10 +2595,10 @@
         <v>1</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q15" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="12">
         <v>220</v>
@@ -2644,24 +2644,24 @@
         <v>1</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q16" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="22"/>
       <c r="C17" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="12">
         <v>220</v>
@@ -2697,10 +2697,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q17" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="Q17" s="21" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2720,12 +2720,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2871,6 +2865,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -2880,22 +2880,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2911,4 +2895,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust (de)comYear to Year(De)Com in PowerBusInfo -> v0.0.4r
Fix change-log formatting
</commit_message>
<xml_diff>
--- a/examples/Power_BusInfo.xlsx
+++ b/examples/Power_BusInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDAE8F6-268A-456C-8EE0-6971AB99BA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDFF1BC-7F2D-4430-BCA3-E793677D0031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarioA" sheetId="111" r:id="rId1"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="80">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -394,12 +394,6 @@
     <t>Decommission Year</t>
   </si>
   <si>
-    <t>comYear</t>
-  </si>
-  <si>
-    <t>decomYear</t>
-  </si>
-  <si>
     <t>[db-key]</t>
   </si>
   <si>
@@ -490,7 +484,16 @@
     <t>Susceptance B connected to node</t>
   </si>
   <si>
-    <t>v0.0.3r</t>
+    <t>YearCom</t>
+  </si>
+  <si>
+    <t>YearDecom</t>
+  </si>
+  <si>
+    <t>excl</t>
+  </si>
+  <si>
+    <t>v0.0.4r</t>
   </si>
 </sst>
 </file>
@@ -1140,15 +1143,15 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>18</v>
@@ -1190,18 +1193,18 @@
         <v>41</v>
       </c>
       <c r="O3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="Q3" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>19</v>
@@ -1230,11 +1233,11 @@
       <c r="J4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>47</v>
+      <c r="K4" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>14</v>
@@ -1243,13 +1246,13 @@
         <v>41</v>
       </c>
       <c r="O4" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="15" t="s">
-        <v>56</v>
-      </c>
       <c r="Q4" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -1273,7 +1276,7 @@
         <v>34</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>36</v>
@@ -1282,10 +1285,10 @@
         <v>40</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>42</v>
@@ -1294,76 +1297,76 @@
         <v>43</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>64</v>
-      </c>
       <c r="L6" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>3</v>
@@ -1396,13 +1399,13 @@
         <v>16</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1412,7 +1415,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="12">
         <v>220</v>
@@ -1448,10 +1451,10 @@
         <v>1</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1461,7 +1464,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="12">
         <v>220</v>
@@ -1497,10 +1500,10 @@
         <v>1</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q9" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -1512,7 +1515,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="12">
         <v>220</v>
@@ -1548,10 +1551,10 @@
         <v>1</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
@@ -1563,7 +1566,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" s="12">
         <v>220</v>
@@ -1599,10 +1602,10 @@
         <v>1</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1612,7 +1615,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12" s="12">
         <v>220</v>
@@ -1648,10 +1651,10 @@
         <v>1</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1661,7 +1664,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E13" s="12">
         <v>220</v>
@@ -1697,10 +1700,10 @@
         <v>1</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1710,7 +1713,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="12">
         <v>220</v>
@@ -1746,10 +1749,10 @@
         <v>1</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q14" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1759,7 +1762,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" s="12">
         <v>220</v>
@@ -1795,10 +1798,10 @@
         <v>1</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q15" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1808,7 +1811,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" s="12">
         <v>220</v>
@@ -1844,24 +1847,24 @@
         <v>1</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q16" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="22"/>
       <c r="C17" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="12">
         <v>220</v>
@@ -1897,10 +1900,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q17" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1919,9 +1922,8 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="H6" sqref="H6"/>
-      <selection pane="topRight" activeCell="H6" sqref="H6"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -1940,15 +1942,15 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>18</v>
@@ -1990,18 +1992,18 @@
         <v>41</v>
       </c>
       <c r="O3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="Q3" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>19</v>
@@ -2031,10 +2033,10 @@
         <v>39</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>14</v>
@@ -2043,13 +2045,13 @@
         <v>41</v>
       </c>
       <c r="O4" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="15" t="s">
-        <v>56</v>
-      </c>
       <c r="Q4" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -2073,7 +2075,7 @@
         <v>34</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>36</v>
@@ -2082,10 +2084,10 @@
         <v>40</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>42</v>
@@ -2094,76 +2096,76 @@
         <v>43</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>64</v>
-      </c>
       <c r="L6" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>3</v>
@@ -2196,13 +2198,13 @@
         <v>16</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -2212,7 +2214,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="12">
         <v>220</v>
@@ -2248,10 +2250,10 @@
         <v>1</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2261,7 +2263,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="12">
         <v>220</v>
@@ -2297,10 +2299,10 @@
         <v>1</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q9" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -2312,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="12">
         <v>220</v>
@@ -2348,10 +2350,10 @@
         <v>1</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q10" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
@@ -2363,7 +2365,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" s="12">
         <v>220</v>
@@ -2399,10 +2401,10 @@
         <v>0</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q11" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2412,7 +2414,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12" s="12">
         <v>220</v>
@@ -2448,10 +2450,10 @@
         <v>0</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2461,7 +2463,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E13" s="12">
         <v>220</v>
@@ -2497,10 +2499,10 @@
         <v>0</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2510,7 +2512,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="12">
         <v>220</v>
@@ -2546,10 +2548,10 @@
         <v>0</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q14" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2559,7 +2561,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" s="12">
         <v>220</v>
@@ -2595,10 +2597,10 @@
         <v>1</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q15" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2608,7 +2610,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" s="12">
         <v>220</v>
@@ -2644,24 +2646,24 @@
         <v>1</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q16" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="22"/>
       <c r="C17" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="12">
         <v>220</v>
@@ -2697,10 +2699,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q17" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2720,6 +2722,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2865,12 +2873,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -2880,6 +2882,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2895,20 +2913,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust scenarionames in Power_BusInfo and Power_Network
</commit_message>
<xml_diff>
--- a/examples/Power_BusInfo.xlsx
+++ b/examples/Power_BusInfo.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDFF1BC-7F2D-4430-BCA3-E793677D0031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D93575A-A2BE-4242-850C-0FCB82917F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scenarioA" sheetId="111" r:id="rId1"/>
-    <sheet name="scenarioB" sheetId="112" r:id="rId2"/>
+    <sheet name="ScenarioA" sheetId="111" r:id="rId1"/>
+    <sheet name="ScenarioB" sheetId="112" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarioA!$L$9:$S$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">scenarioB!$L$9:$S$16</definedName>
-    <definedName name="businfo" localSheetId="1">scenarioB!$B$3:$O$16</definedName>
-    <definedName name="businfo">scenarioA!$B$3:$O$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ScenarioA!$L$9:$S$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ScenarioB!$L$9:$S$16</definedName>
+    <definedName name="businfo" localSheetId="1">ScenarioB!$B$3:$O$16</definedName>
+    <definedName name="businfo">ScenarioA!$B$3:$O$16</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
     <definedName name="dsmprofiles">#REF!</definedName>
@@ -1187,10 +1187,10 @@
         <v>45</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>51</v>
@@ -1986,10 +1986,10 @@
         <v>45</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>51</v>
@@ -2722,12 +2722,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2873,6 +2867,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -2882,22 +2882,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2913,4 +2897,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust column widths and descriptions for most columns (and thus files)
</commit_message>
<xml_diff>
--- a/examples/Power_BusInfo.xlsx
+++ b/examples/Power_BusInfo.xlsx
@@ -244,9 +244,7 @@
   <commentList>
     <comment ref="A3" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">
-            If a line has a value in this column, it is not read in (i.e., does not exist).
-        </t>
+        <t>If a line has a value in this column, it is not read in (i.e., does not exist).</t>
       </text>
     </comment>
     <comment ref="B3" authorId="0" shapeId="0">
@@ -286,9 +284,7 @@
   <commentList>
     <comment ref="A3" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">
-            If a line has a value in this column, it is not read in (i.e., does not exist).
-        </t>
+        <t>If a line has a value in this column, it is not read in (i.e., does not exist).</t>
       </text>
     </comment>
     <comment ref="B3" authorId="0" shapeId="0">
@@ -622,20 +618,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="5.5709375" customWidth="1" min="1" max="1"/>
-    <col width="20.2809375" customWidth="1" min="2" max="2"/>
+    <col width="19.7109375" customWidth="1" min="2" max="2"/>
     <col width="15.7109375" customWidth="1" min="3" max="3"/>
     <col width="15.7109375" customWidth="1" min="4" max="4"/>
-    <col width="19.7109375" customWidth="1" min="5" max="5"/>
-    <col width="20.7109375" customWidth="1" min="6" max="6"/>
-    <col width="20.7109375" customWidth="1" min="7" max="7"/>
-    <col width="20.7109375" customWidth="1" min="8" max="8"/>
-    <col width="20.7109375" customWidth="1" min="9" max="9"/>
-    <col width="20.7109375" customWidth="1" min="10" max="10"/>
+    <col width="15.7109375" customWidth="1" min="5" max="5"/>
+    <col width="15.7109375" customWidth="1" min="6" max="6"/>
+    <col width="15.7109375" customWidth="1" min="7" max="7"/>
+    <col width="15.7109375" customWidth="1" min="8" max="8"/>
+    <col width="15.7109375" customWidth="1" min="9" max="9"/>
+    <col width="15.7109375" customWidth="1" min="10" max="10"/>
     <col width="20.2109375" customWidth="1" min="11" max="11"/>
     <col width="20.2109375" customWidth="1" min="12" max="12"/>
     <col width="15.7109375" customWidth="1" min="13" max="13"/>
     <col width="15.7109375" customWidth="1" min="14" max="14"/>
-    <col width="20.0109375" customWidth="1" min="15" max="15"/>
+    <col width="18.7109375" customWidth="1" min="15" max="15"/>
     <col width="24.5709375" customWidth="1" min="16" max="16"/>
     <col width="24.5709375" customWidth="1" min="17" max="17"/>
   </cols>
@@ -671,7 +667,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.1</t>
+          <t>v0.1.2</t>
         </is>
       </c>
     </row>
@@ -873,7 +869,7 @@
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
-          <t>Maximum voltage (in % of bae voltage)</t>
+          <t>Maximum voltage (in % of base voltage)</t>
         </is>
       </c>
       <c r="G5" s="7" t="inlineStr">
@@ -1717,20 +1713,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="5.5709375" customWidth="1" min="1" max="1"/>
-    <col width="20.2809375" customWidth="1" min="2" max="2"/>
+    <col width="19.7109375" customWidth="1" min="2" max="2"/>
     <col width="15.7109375" customWidth="1" min="3" max="3"/>
     <col width="15.7109375" customWidth="1" min="4" max="4"/>
-    <col width="19.7109375" customWidth="1" min="5" max="5"/>
-    <col width="20.7109375" customWidth="1" min="6" max="6"/>
-    <col width="20.7109375" customWidth="1" min="7" max="7"/>
-    <col width="20.7109375" customWidth="1" min="8" max="8"/>
-    <col width="20.7109375" customWidth="1" min="9" max="9"/>
-    <col width="20.7109375" customWidth="1" min="10" max="10"/>
+    <col width="15.7109375" customWidth="1" min="5" max="5"/>
+    <col width="15.7109375" customWidth="1" min="6" max="6"/>
+    <col width="15.7109375" customWidth="1" min="7" max="7"/>
+    <col width="15.7109375" customWidth="1" min="8" max="8"/>
+    <col width="15.7109375" customWidth="1" min="9" max="9"/>
+    <col width="15.7109375" customWidth="1" min="10" max="10"/>
     <col width="20.2109375" customWidth="1" min="11" max="11"/>
     <col width="20.2109375" customWidth="1" min="12" max="12"/>
     <col width="15.7109375" customWidth="1" min="13" max="13"/>
     <col width="15.7109375" customWidth="1" min="14" max="14"/>
-    <col width="20.0109375" customWidth="1" min="15" max="15"/>
+    <col width="18.7109375" customWidth="1" min="15" max="15"/>
     <col width="24.5709375" customWidth="1" min="16" max="16"/>
     <col width="24.5709375" customWidth="1" min="17" max="17"/>
   </cols>
@@ -1766,7 +1762,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.1</t>
+          <t>v0.1.2</t>
         </is>
       </c>
     </row>
@@ -1968,7 +1964,7 @@
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
-          <t>Maximum voltage (in % of bae voltage)</t>
+          <t>Maximum voltage (in % of base voltage)</t>
         </is>
       </c>
       <c r="G5" s="7" t="inlineStr">

</xml_diff>